<commit_message>
update files for patients with missing last sample collection dates
</commit_message>
<xml_diff>
--- a/Datasets/bl_eos_arg_counts.xlsx
+++ b/Datasets/bl_eos_arg_counts.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinaramont/Documents/research for dr.g-p/my created datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinaramont/galloway_lab/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3228D3C4-2B71-FF4C-B16C-8E6434E9CE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B0F79C-4D9E-F445-AFD5-F84CC1F3213E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{85B7FDAF-796C-734F-838C-A347400AAEF2}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{85B7FDAF-796C-734F-838C-A347400AAEF2}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
     <sheet name="collection_info" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="collection_info_complete" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="170">
   <si>
     <t>cohort</t>
   </si>
@@ -545,6 +546,9 @@
   </si>
   <si>
     <t>15-0780-060</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -609,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -619,8 +623,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,15 +649,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
+      <xdr:colOff>215899</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28863</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>187613</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -666,8 +672,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="215900" y="381000"/>
-          <a:ext cx="10414000" cy="7429500"/>
+          <a:off x="215899" y="379845"/>
+          <a:ext cx="10506941" cy="9505950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -762,6 +768,15 @@
           <a:r>
             <a:rPr lang="en-US" sz="2400" baseline="0"/>
             <a:t>" which was provided to me by Dr. G.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2400" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" baseline="0"/>
+            <a:t>The tab "collection_info" includes the patients included in the analyses for BL and EOS ARG counts since they have last sample collection dates available. The tab "collection_info_complete" has all the patients, even those with missing last sample collection dates (specifically 0339-2013-085).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1089,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE369CD-FF73-C04F-8138-9CA87979B9A2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1102,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E50FAEB-D9CA-8C40-B6DB-614E161CA699}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView zoomScale="158" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,49 +1181,55 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="5">
+      <c r="F3" s="10">
+        <v>41621</v>
+      </c>
+      <c r="G3" s="8">
         <v>150</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G4" s="5">
+      <c r="F4" s="10">
+        <v>41635</v>
+      </c>
+      <c r="G4" s="8">
         <v>51</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="8">
         <v>71</v>
       </c>
     </row>
@@ -1502,7 +1523,7 @@
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="1">
         <v>61</v>
       </c>
       <c r="C16" t="s">
@@ -1628,27 +1649,30 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="5">
-        <v>85</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="G21" s="5">
-        <v>117</v>
-      </c>
-      <c r="H21" s="5">
-        <v>74</v>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="4">
+        <v>42096</v>
+      </c>
+      <c r="G21" s="1">
+        <v>54</v>
+      </c>
+      <c r="H21" s="1">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1656,25 +1680,25 @@
         <v>4</v>
       </c>
       <c r="B22" s="1">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E22" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F22" s="4">
-        <v>42096</v>
+        <v>42157</v>
       </c>
       <c r="G22" s="1">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="H22" s="1">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1682,25 +1706,25 @@
         <v>4</v>
       </c>
       <c r="B23" s="1">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F23" s="4">
-        <v>42157</v>
+        <v>42546</v>
       </c>
       <c r="G23" s="1">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="H23" s="1">
-        <v>57</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1708,25 +1732,25 @@
         <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F24" s="4">
-        <v>42546</v>
+        <v>42229</v>
       </c>
       <c r="G24" s="1">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="H24" s="1">
-        <v>101</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1734,25 +1758,25 @@
         <v>4</v>
       </c>
       <c r="B25" s="1">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F25" s="4">
-        <v>42229</v>
+        <v>42215</v>
       </c>
       <c r="G25" s="1">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="H25" s="1">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1760,51 +1784,51 @@
         <v>4</v>
       </c>
       <c r="B26" s="1">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E26" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F26" s="4">
-        <v>42215</v>
+        <v>42227</v>
       </c>
       <c r="G26" s="1">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="H26" s="1">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" s="1">
-        <v>101</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>147</v>
+        <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="F27" s="4">
-        <v>42227</v>
+        <v>42381</v>
       </c>
       <c r="G27" s="1">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="H27" s="1">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1812,25 +1836,25 @@
         <v>5</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F28" s="4">
-        <v>42381</v>
+        <v>42538</v>
       </c>
       <c r="G28" s="1">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="H28" s="1">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1838,25 +1862,25 @@
         <v>5</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>156</v>
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F29" s="4">
-        <v>42538</v>
+        <v>42409</v>
       </c>
       <c r="G29" s="1">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="H29" s="1">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1864,25 +1888,25 @@
         <v>5</v>
       </c>
       <c r="B30" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F30" s="4">
-        <v>42409</v>
+        <v>42150</v>
       </c>
       <c r="G30" s="1">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="H30" s="1">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1890,25 +1914,25 @@
         <v>5</v>
       </c>
       <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F31" s="4">
-        <v>42150</v>
+        <v>42535</v>
       </c>
       <c r="G31" s="1">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="H31" s="1">
-        <v>86</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1916,25 +1940,25 @@
         <v>5</v>
       </c>
       <c r="B32" s="1">
-        <v>12</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>151</v>
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F32" s="4">
-        <v>42535</v>
+        <v>42675</v>
       </c>
       <c r="G32" s="1">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="H32" s="1">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1942,25 +1966,25 @@
         <v>5</v>
       </c>
       <c r="B33" s="1">
-        <v>14</v>
-      </c>
-      <c r="C33" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F33" s="4">
-        <v>42675</v>
+        <v>42542</v>
       </c>
       <c r="G33" s="1">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="H33" s="1">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1968,51 +1992,51 @@
         <v>5</v>
       </c>
       <c r="B34" s="1">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E34" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F34" s="4">
-        <v>42542</v>
+        <v>42689</v>
       </c>
       <c r="G34" s="1">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H34" s="1">
-        <v>77</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="8">
-        <v>25</v>
+      <c r="B35" s="1">
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F35" s="4">
-        <v>42689</v>
+        <v>42797</v>
       </c>
       <c r="G35" s="1">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="H35" s="1">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -2020,25 +2044,25 @@
         <v>5</v>
       </c>
       <c r="B36" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F36" s="4">
-        <v>42797</v>
+        <v>42886</v>
       </c>
       <c r="G36" s="1">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="H36" s="1">
-        <v>28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -2046,25 +2070,25 @@
         <v>5</v>
       </c>
       <c r="B37" s="1">
-        <v>29</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>155</v>
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E37" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F37" s="4">
         <v>42886</v>
       </c>
       <c r="G37" s="1">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="H37" s="1">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -2072,25 +2096,25 @@
         <v>5</v>
       </c>
       <c r="B38" s="1">
-        <v>30</v>
-      </c>
-      <c r="C38" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E38" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F38" s="4">
         <v>42886</v>
       </c>
       <c r="G38" s="1">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H38" s="1">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -2098,25 +2122,25 @@
         <v>5</v>
       </c>
       <c r="B39" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="4">
+        <v>42900</v>
+      </c>
+      <c r="G39" s="1">
+        <v>23</v>
+      </c>
+      <c r="H39" s="1">
         <v>65</v>
-      </c>
-      <c r="F39" s="4">
-        <v>42886</v>
-      </c>
-      <c r="G39" s="1">
-        <v>76</v>
-      </c>
-      <c r="H39" s="1">
-        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -2124,25 +2148,25 @@
         <v>5</v>
       </c>
       <c r="B40" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E40" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F40" s="4">
-        <v>42900</v>
+        <v>43067</v>
       </c>
       <c r="G40" s="1">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="H40" s="1">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -2150,25 +2174,25 @@
         <v>5</v>
       </c>
       <c r="B41" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F41" s="4">
-        <v>43067</v>
+        <v>71</v>
+      </c>
+      <c r="F41" s="7">
+        <v>43011</v>
       </c>
       <c r="G41" s="1">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="H41" s="1">
-        <v>84</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -2176,25 +2200,25 @@
         <v>5</v>
       </c>
       <c r="B42" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D42" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" s="7">
-        <v>43011</v>
+        <v>73</v>
+      </c>
+      <c r="F42" s="4">
+        <v>43105</v>
       </c>
       <c r="G42" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H42" s="1">
-        <v>31</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -2202,25 +2226,25 @@
         <v>5</v>
       </c>
       <c r="B43" s="1">
-        <v>38</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>160</v>
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F43" s="4">
-        <v>43105</v>
+        <v>43172</v>
       </c>
       <c r="G43" s="1">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="H43" s="1">
-        <v>84</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -2228,25 +2252,25 @@
         <v>5</v>
       </c>
       <c r="B44" s="1">
-        <v>40</v>
-      </c>
-      <c r="C44" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="D44" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F44" s="4">
-        <v>43172</v>
+        <v>43550</v>
       </c>
       <c r="G44" s="1">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="H44" s="1">
-        <v>120</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2254,25 +2278,25 @@
         <v>5</v>
       </c>
       <c r="B45" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E45" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F45" s="4">
-        <v>43550</v>
+        <v>43579</v>
       </c>
       <c r="G45" s="1">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H45" s="1">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -2280,25 +2304,25 @@
         <v>5</v>
       </c>
       <c r="B46" s="1">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D46" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F46" s="4">
-        <v>43579</v>
+        <v>43706</v>
       </c>
       <c r="G46" s="1">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="H46" s="1">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2306,25 +2330,25 @@
         <v>5</v>
       </c>
       <c r="B47" s="1">
-        <v>48</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>163</v>
+        <v>51</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F47" s="4">
-        <v>43706</v>
+        <v>43712</v>
       </c>
       <c r="G47" s="1">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H47" s="1">
-        <v>96</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2332,25 +2356,25 @@
         <v>5</v>
       </c>
       <c r="B48" s="1">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E48" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F48" s="4">
-        <v>43712</v>
+        <v>43788</v>
       </c>
       <c r="G48" s="1">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H48" s="1">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2358,25 +2382,25 @@
         <v>5</v>
       </c>
       <c r="B49" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D49" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F49" s="4">
-        <v>43788</v>
+        <v>43795</v>
       </c>
       <c r="G49" s="1">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="H49" s="1">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2384,25 +2408,25 @@
         <v>5</v>
       </c>
       <c r="B50" s="1">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F50" s="4">
-        <v>43795</v>
+        <v>43822</v>
       </c>
       <c r="G50" s="1">
         <v>42</v>
       </c>
       <c r="H50" s="1">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2410,25 +2434,25 @@
         <v>5</v>
       </c>
       <c r="B51" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D51" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E51" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F51" s="4">
-        <v>43822</v>
+        <v>43865</v>
       </c>
       <c r="G51" s="1">
-        <v>42</v>
+        <v>145</v>
       </c>
       <c r="H51" s="1">
-        <v>58</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2436,25 +2460,25 @@
         <v>5</v>
       </c>
       <c r="B52" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E52" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F52" s="4">
-        <v>43865</v>
+        <v>43852</v>
       </c>
       <c r="G52" s="1">
-        <v>145</v>
+        <v>54</v>
       </c>
       <c r="H52" s="1">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2462,50 +2486,24 @@
         <v>5</v>
       </c>
       <c r="B53" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D53" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F53" s="4">
-        <v>43852</v>
+        <v>43865</v>
       </c>
       <c r="G53" s="1">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="H53" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="1">
-        <v>63</v>
-      </c>
-      <c r="C54" t="s">
-        <v>165</v>
-      </c>
-      <c r="D54" t="s">
-        <v>94</v>
-      </c>
-      <c r="E54" t="s">
-        <v>95</v>
-      </c>
-      <c r="F54" s="4">
-        <v>43865</v>
-      </c>
-      <c r="G54" s="1">
-        <v>88</v>
-      </c>
-      <c r="H54" s="1">
         <v>83</v>
       </c>
     </row>
@@ -2515,6 +2513,1425 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADF080-A197-7342-9821-9D8A79F580AB}">
+  <dimension ref="A1:H54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="4">
+        <v>41612</v>
+      </c>
+      <c r="G2" s="1">
+        <v>47</v>
+      </c>
+      <c r="H2" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8">
+        <v>10</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="10">
+        <v>41621</v>
+      </c>
+      <c r="G3" s="8">
+        <v>150</v>
+      </c>
+      <c r="H3" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="10">
+        <v>41635</v>
+      </c>
+      <c r="G4" s="8">
+        <v>51</v>
+      </c>
+      <c r="H4" s="8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="4">
+        <v>41643</v>
+      </c>
+      <c r="G5" s="1">
+        <v>99</v>
+      </c>
+      <c r="H5" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="4">
+        <v>41666</v>
+      </c>
+      <c r="G6" s="1">
+        <v>98</v>
+      </c>
+      <c r="H6" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="4">
+        <v>41691</v>
+      </c>
+      <c r="G7" s="1">
+        <v>67</v>
+      </c>
+      <c r="H7" s="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="4">
+        <v>41697</v>
+      </c>
+      <c r="G8" s="1">
+        <v>52</v>
+      </c>
+      <c r="H8" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="4">
+        <v>41754</v>
+      </c>
+      <c r="G9" s="1">
+        <v>131</v>
+      </c>
+      <c r="H9" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="4">
+        <v>41817</v>
+      </c>
+      <c r="G10" s="1">
+        <v>75</v>
+      </c>
+      <c r="H10" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="4">
+        <v>41828</v>
+      </c>
+      <c r="G11" s="1">
+        <v>55</v>
+      </c>
+      <c r="H11" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="4">
+        <v>41849</v>
+      </c>
+      <c r="G12" s="1">
+        <v>98</v>
+      </c>
+      <c r="H12" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="4">
+        <v>41879</v>
+      </c>
+      <c r="G13" s="1">
+        <v>77</v>
+      </c>
+      <c r="H13" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="4">
+        <v>41879</v>
+      </c>
+      <c r="G14" s="1">
+        <v>103</v>
+      </c>
+      <c r="H14" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="4">
+        <v>41905</v>
+      </c>
+      <c r="G15" s="1">
+        <v>61</v>
+      </c>
+      <c r="H15" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" s="4">
+        <v>41920</v>
+      </c>
+      <c r="G16" s="1">
+        <v>103</v>
+      </c>
+      <c r="H16" s="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="4">
+        <v>41936</v>
+      </c>
+      <c r="G17" s="1">
+        <v>35</v>
+      </c>
+      <c r="H17" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="4">
+        <v>41942</v>
+      </c>
+      <c r="G18" s="1">
+        <v>98</v>
+      </c>
+      <c r="H18" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="4">
+        <v>42017</v>
+      </c>
+      <c r="G19" s="1">
+        <v>29</v>
+      </c>
+      <c r="H19" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="4">
+        <v>42054</v>
+      </c>
+      <c r="G20" s="1">
+        <v>99</v>
+      </c>
+      <c r="H20" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5">
+        <v>85</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G21" s="5">
+        <v>117</v>
+      </c>
+      <c r="H21" s="5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="4">
+        <v>42096</v>
+      </c>
+      <c r="G22" s="1">
+        <v>54</v>
+      </c>
+      <c r="H22" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>93</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="4">
+        <v>42157</v>
+      </c>
+      <c r="G23" s="1">
+        <v>120</v>
+      </c>
+      <c r="H23" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1">
+        <v>95</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24" s="4">
+        <v>42546</v>
+      </c>
+      <c r="G24" s="1">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="4">
+        <v>42229</v>
+      </c>
+      <c r="G25" s="1">
+        <v>107</v>
+      </c>
+      <c r="H25" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="4">
+        <v>42215</v>
+      </c>
+      <c r="G26" s="1">
+        <v>140</v>
+      </c>
+      <c r="H26" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1">
+        <v>101</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="4">
+        <v>42227</v>
+      </c>
+      <c r="G27" s="1">
+        <v>114</v>
+      </c>
+      <c r="H27" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="4">
+        <v>42381</v>
+      </c>
+      <c r="G28" s="1">
+        <v>95</v>
+      </c>
+      <c r="H28" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="4">
+        <v>42538</v>
+      </c>
+      <c r="G29" s="1">
+        <v>108</v>
+      </c>
+      <c r="H29" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="4">
+        <v>42409</v>
+      </c>
+      <c r="G30" s="1">
+        <v>53</v>
+      </c>
+      <c r="H30" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="4">
+        <v>42150</v>
+      </c>
+      <c r="G31" s="1">
+        <v>117</v>
+      </c>
+      <c r="H31" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="4">
+        <v>42535</v>
+      </c>
+      <c r="G32" s="1">
+        <v>83</v>
+      </c>
+      <c r="H32" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="4">
+        <v>42675</v>
+      </c>
+      <c r="G33" s="1">
+        <v>93</v>
+      </c>
+      <c r="H33" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1">
+        <v>18</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="4">
+        <v>42542</v>
+      </c>
+      <c r="G34" s="1">
+        <v>55</v>
+      </c>
+      <c r="H34" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1">
+        <v>25</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="4">
+        <v>42689</v>
+      </c>
+      <c r="G35" s="1">
+        <v>61</v>
+      </c>
+      <c r="H35" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1">
+        <v>26</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="4">
+        <v>42797</v>
+      </c>
+      <c r="G36" s="1">
+        <v>86</v>
+      </c>
+      <c r="H36" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1">
+        <v>29</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="4">
+        <v>42886</v>
+      </c>
+      <c r="G37" s="1">
+        <v>115</v>
+      </c>
+      <c r="H37" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" t="s">
+        <v>63</v>
+      </c>
+      <c r="F38" s="4">
+        <v>42886</v>
+      </c>
+      <c r="G38" s="1">
+        <v>78</v>
+      </c>
+      <c r="H38" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1">
+        <v>31</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="4">
+        <v>42886</v>
+      </c>
+      <c r="G39" s="1">
+        <v>76</v>
+      </c>
+      <c r="H39" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1">
+        <v>33</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="4">
+        <v>42900</v>
+      </c>
+      <c r="G40" s="1">
+        <v>23</v>
+      </c>
+      <c r="H40" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1">
+        <v>35</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="4">
+        <v>43067</v>
+      </c>
+      <c r="G41" s="1">
+        <v>5</v>
+      </c>
+      <c r="H41" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1">
+        <v>37</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D42" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="7">
+        <v>43011</v>
+      </c>
+      <c r="G42" s="1">
+        <v>79</v>
+      </c>
+      <c r="H42" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1">
+        <v>38</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="4">
+        <v>43105</v>
+      </c>
+      <c r="G43" s="1">
+        <v>80</v>
+      </c>
+      <c r="H43" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="1">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" s="4">
+        <v>43172</v>
+      </c>
+      <c r="G44" s="1">
+        <v>67</v>
+      </c>
+      <c r="H44" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1">
+        <v>41</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="4">
+        <v>43550</v>
+      </c>
+      <c r="G45" s="1">
+        <v>90</v>
+      </c>
+      <c r="H45" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" s="4">
+        <v>43579</v>
+      </c>
+      <c r="G46" s="1">
+        <v>85</v>
+      </c>
+      <c r="H46" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="1">
+        <v>48</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" s="4">
+        <v>43706</v>
+      </c>
+      <c r="G47" s="1">
+        <v>71</v>
+      </c>
+      <c r="H47" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="1">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="4">
+        <v>43712</v>
+      </c>
+      <c r="G48" s="1">
+        <v>61</v>
+      </c>
+      <c r="H48" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="4">
+        <v>43788</v>
+      </c>
+      <c r="G49" s="1">
+        <v>75</v>
+      </c>
+      <c r="H49" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="1">
+        <v>56</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" s="4">
+        <v>43795</v>
+      </c>
+      <c r="G50" s="1">
+        <v>42</v>
+      </c>
+      <c r="H50" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1">
+        <v>60</v>
+      </c>
+      <c r="C51" t="s">
+        <v>168</v>
+      </c>
+      <c r="D51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="4">
+        <v>43822</v>
+      </c>
+      <c r="G51" s="1">
+        <v>42</v>
+      </c>
+      <c r="H51" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1">
+        <v>61</v>
+      </c>
+      <c r="C52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" t="s">
+        <v>91</v>
+      </c>
+      <c r="F52" s="4">
+        <v>43865</v>
+      </c>
+      <c r="G52" s="1">
+        <v>145</v>
+      </c>
+      <c r="H52" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="1">
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="4">
+        <v>43852</v>
+      </c>
+      <c r="G53" s="1">
+        <v>54</v>
+      </c>
+      <c r="H53" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1">
+        <v>63</v>
+      </c>
+      <c r="C54" t="s">
+        <v>165</v>
+      </c>
+      <c r="D54" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="4">
+        <v>43865</v>
+      </c>
+      <c r="G54" s="1">
+        <v>88</v>
+      </c>
+      <c r="H54" s="1">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC292404-4B45-614A-A948-E2C7F1DACEF0}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>